<commit_message>
Update CLass Diagram e matrice
</commit_message>
<xml_diff>
--- a/DocumentazioneODD/Check_List_ODD.xlsx
+++ b/DocumentazioneODD/Check_List_ODD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lciri\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ciro\Desktop\IS\NewDM\DocumentazioneODD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE46150-7417-420C-834B-EDC3F925A071}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DFE5CD-A7B0-4E06-8C33-50EE377D89DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="646" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="646" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Check-list ODD" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="57">
   <si>
     <t>N° linee guida soddisfatte</t>
   </si>
@@ -79,19 +78,6 @@
     <t>Check List ODD</t>
   </si>
   <si>
-    <t>Progetto: &lt;Id Progetto&gt;</t>
-  </si>
-  <si>
-    <t>Autore del controllo:
-&lt;Cognome Nome&gt;</t>
-  </si>
-  <si>
-    <t>Data: gg/mm/aa</t>
-  </si>
-  <si>
-    <t>Versione Documento</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -111,12 +97,6 @@
   </si>
   <si>
     <t>SI</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>L’Indice dei Contenuti è aggiornato, riportando le intestazioni di tutti i capitoli, paragrafi e sottoparagrafi presenti nel corpo del documento, puntando correttamente alle sezioni relative?</t>
@@ -244,6 +224,19 @@
   </si>
   <si>
     <t>E' rispettato sia per le classi sia per Javadoc lo standard di codifica adottato per la verifica con checkstyle?</t>
+  </si>
+  <si>
+    <t>Progetto: NC_09</t>
+  </si>
+  <si>
+    <t>Autore del controllo: FUSCO CIRO
+&lt;Cognome Nome&gt;</t>
+  </si>
+  <si>
+    <t>Data: 03/02/2021</t>
+  </si>
+  <si>
+    <t>Poiché javadoc non prevede più luso di @pre e @post, sono state uaste descrizioni letterali al loro posto</t>
   </si>
 </sst>
 </file>
@@ -900,25 +893,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -927,17 +902,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -967,6 +951,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1005,6 +992,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1017,14 +1044,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1039,69 +1090,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1467,21 +1460,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J40"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="6.36328125" customWidth="1"/>
-    <col min="4" max="4" width="68.6328125" customWidth="1"/>
-    <col min="5" max="5" width="6.1796875" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" customWidth="1"/>
+    <col min="4" max="4" width="68.5703125" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="73.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="73.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="38.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" ht="38.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
       <c r="D1" s="34" t="s">
@@ -1490,17 +1483,17 @@
       <c r="E1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="59" t="s">
+      <c r="F1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="61"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="58"/>
       <c r="J1" s="36" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B2" s="44"/>
       <c r="C2" s="44"/>
       <c r="D2" s="8">
@@ -1509,21 +1502,21 @@
       </c>
       <c r="E2" s="5">
         <f>COUNTIF(E15:E40, "NA")</f>
-        <v>13</v>
+        <v>0</v>
       </c>
-      <c r="F2" s="62">
+      <c r="F2" s="59">
         <f>COUNTIF(F15:I40, "NO")</f>
-        <v>13</v>
+        <v>0</v>
       </c>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
       <c r="J2" s="9" t="str">
         <f>IF((D2+E2+F2)=53, OK, "Controlla se hai cancellato tutte le voci che non servono e se hai dato tutte le risposte")</f>
         <v>Controlla se hai cancellato tutte le voci che non servono e se hai dato tutte le risposte</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="45"/>
       <c r="C3" s="45"/>
       <c r="D3" s="10"/>
@@ -1544,33 +1537,33 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="45"/>
       <c r="C4" s="45"/>
       <c r="D4" s="11"/>
       <c r="E4" s="12"/>
       <c r="F4" s="13">
         <f>COUNTIF(F15:I40, F3)</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G4" s="13">
         <f>COUNTIF(F15:I40, G3)</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="H4" s="13">
         <f>COUNTIF(F15:I40, H3)</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="I4" s="23">
         <f>COUNTIF(F15:I40, I3)</f>
-        <v>13</v>
+        <v>0</v>
       </c>
-      <c r="J4" s="9" t="str">
+      <c r="J4" s="9" t="e">
         <f>IF((F4+G4+H4)=(F2), OK, "Controlla se hai cancellato tutte le voci che non servono")</f>
-        <v>Controlla se hai cancellato tutte le voci che non servono</v>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B5" s="45"/>
       <c r="C5" s="45"/>
       <c r="D5" s="45"/>
@@ -1581,20 +1574,20 @@
       <c r="I5" s="45"/>
       <c r="J5" s="45"/>
     </row>
-    <row r="6" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="45"/>
       <c r="C6" s="45"/>
-      <c r="D6" s="79" t="s">
+      <c r="D6" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="80"/>
-      <c r="F6" s="80"/>
-      <c r="G6" s="80"/>
-      <c r="H6" s="80"/>
-      <c r="I6" s="80"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="78"/>
+      <c r="I6" s="78"/>
       <c r="J6" s="45"/>
     </row>
-    <row r="8" spans="2:10" ht="20" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:10" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B8" s="45"/>
       <c r="C8" s="45"/>
       <c r="D8" s="1" t="s">
@@ -1607,7 +1600,7 @@
       <c r="I8" s="45"/>
       <c r="J8" s="45"/>
     </row>
-    <row r="9" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B9" s="44"/>
       <c r="C9" s="44"/>
       <c r="D9" s="44"/>
@@ -1618,618 +1611,473 @@
       <c r="I9" s="44"/>
       <c r="J9" s="44"/>
     </row>
-    <row r="10" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:10" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="44"/>
-      <c r="C10" s="77" t="s">
-        <v>7</v>
+      <c r="C10" s="75" t="s">
+        <v>53</v>
       </c>
-      <c r="D10" s="78"/>
-      <c r="E10" s="72" t="s">
-        <v>8</v>
+      <c r="D10" s="76"/>
+      <c r="E10" s="70" t="s">
+        <v>54</v>
       </c>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="74"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="72"/>
       <c r="J10" s="2" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:10" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="44"/>
-      <c r="C11" s="71" t="s">
-        <v>10</v>
+      <c r="C11" s="69">
+        <v>1</v>
       </c>
-      <c r="D11" s="71"/>
+      <c r="D11" s="69"/>
       <c r="E11" s="38"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="81"/>
-      <c r="I11" s="81"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="79"/>
       <c r="J11" s="32"/>
     </row>
-    <row r="12" spans="2:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B12" s="44"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="76"/>
-      <c r="I12" s="76"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="74"/>
+      <c r="I12" s="74"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="44"/>
       <c r="C13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" s="15" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="44"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="66"/>
+    </row>
+    <row r="15" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="44"/>
+      <c r="C15" s="49">
+        <v>1</v>
+      </c>
+      <c r="D15" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="65" t="s">
+      <c r="E15" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="4" t="s">
+      <c r="F15" s="80"/>
+      <c r="G15" s="81"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="49"/>
+    </row>
+    <row r="16" spans="2:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="45"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="50"/>
+    </row>
+    <row r="17" spans="2:10" s="24" customFormat="1" ht="43.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="44"/>
+      <c r="C17" s="49">
+        <v>2</v>
+      </c>
+      <c r="D17" s="67" t="s">
         <v>14</v>
       </c>
+      <c r="E17" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="46"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="55"/>
+      <c r="J17" s="49"/>
     </row>
-    <row r="14" spans="2:10" s="15" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="44"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="68" t="s">
+    <row r="18" spans="2:10" s="24" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="44"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="83"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="50"/>
+    </row>
+    <row r="19" spans="2:10" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="44"/>
+      <c r="C19" s="49">
+        <v>3</v>
+      </c>
+      <c r="D19" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="68"/>
-      <c r="H14" s="68"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="69"/>
+      <c r="E19" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="46"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="55"/>
+      <c r="J19" s="41"/>
     </row>
-    <row r="15" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="44"/>
-      <c r="C15" s="46">
-        <v>1</v>
+    <row r="20" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="44"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="83"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="43"/>
+    </row>
+    <row r="21" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="44"/>
+      <c r="C21" s="49">
+        <v>4</v>
       </c>
-      <c r="D15" s="48" t="s">
+      <c r="D21" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E21" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="46"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="49"/>
+    </row>
+    <row r="22" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="44"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="83"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="50"/>
+    </row>
+    <row r="23" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="44"/>
+      <c r="C23" s="49">
+        <v>5</v>
+      </c>
+      <c r="D23" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="82" t="s">
+      <c r="E23" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="46"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="49"/>
+    </row>
+    <row r="24" spans="2:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="44"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="83"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="50"/>
+    </row>
+    <row r="25" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="44"/>
+      <c r="C25" s="49">
+        <v>6</v>
+      </c>
+      <c r="D25" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="83"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="46"/>
+      <c r="E25" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="46"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="49"/>
     </row>
-    <row r="16" spans="2:10" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="45"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="70"/>
-      <c r="E16" s="42" t="s">
+    <row r="26" spans="2:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="44"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="50"/>
+    </row>
+    <row r="27" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="44"/>
+      <c r="C27" s="49">
+        <v>7</v>
+      </c>
+      <c r="D27" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="20">
-        <v>0.1</v>
+      <c r="E27" s="30" t="s">
+        <v>13</v>
       </c>
-      <c r="G16" s="20">
-        <v>0.3</v>
+      <c r="F27" s="46"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="49"/>
+    </row>
+    <row r="28" spans="2:10" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="44"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="83"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="50"/>
+    </row>
+    <row r="29" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="44"/>
+      <c r="C29" s="49">
+        <v>8</v>
       </c>
-      <c r="H16" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="I16" s="20">
-        <v>0.7</v>
-      </c>
-      <c r="J16" s="47"/>
-    </row>
-    <row r="17" spans="2:10" s="24" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="44"/>
-      <c r="C17" s="46">
-        <v>2</v>
-      </c>
-      <c r="D17" s="48" t="s">
+      <c r="D29" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="30" t="s">
-        <v>17</v>
+      <c r="E29" s="30" t="s">
+        <v>13</v>
       </c>
-      <c r="F17" s="50" t="s">
-        <v>18</v>
+      <c r="F29" s="46"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="49"/>
+    </row>
+    <row r="30" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="44"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="83"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="53"/>
+    </row>
+    <row r="31" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="44"/>
+      <c r="C31" s="49">
+        <v>9</v>
       </c>
-      <c r="G17" s="51"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="46"/>
-    </row>
-    <row r="18" spans="2:10" s="24" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="44"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="G18" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="H18" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="I18" s="20">
-        <v>0.7</v>
-      </c>
-      <c r="J18" s="47"/>
-    </row>
-    <row r="19" spans="2:10" ht="38" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="44"/>
-      <c r="C19" s="46">
-        <v>3</v>
-      </c>
-      <c r="D19" s="55" t="s">
+      <c r="D31" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="30" t="s">
-        <v>17</v>
+      <c r="E31" s="30" t="s">
+        <v>13</v>
       </c>
-      <c r="F19" s="50" t="s">
-        <v>18</v>
+      <c r="F31" s="46"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="49"/>
+    </row>
+    <row r="32" spans="2:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="44"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="83"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="50"/>
+    </row>
+    <row r="33" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="44"/>
+      <c r="C33" s="49">
+        <v>10</v>
       </c>
-      <c r="G19" s="51"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="41"/>
-    </row>
-    <row r="20" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="44"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="G20" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="H20" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="I20" s="20">
-        <v>0.7</v>
-      </c>
-      <c r="J20" s="43"/>
-    </row>
-    <row r="21" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="44"/>
-      <c r="C21" s="46">
-        <v>4</v>
-      </c>
-      <c r="D21" s="55" t="s">
+      <c r="D33" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="30" t="s">
-        <v>17</v>
+      <c r="E33" s="30" t="s">
+        <v>13</v>
       </c>
-      <c r="F21" s="50" t="s">
-        <v>18</v>
+      <c r="F33" s="46"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="48"/>
+      <c r="J33" s="49"/>
+    </row>
+    <row r="34" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="44"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="83"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="50"/>
+    </row>
+    <row r="35" spans="2:10" s="27" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="45"/>
+      <c r="C35" s="49">
+        <v>11</v>
       </c>
-      <c r="G21" s="53"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="46"/>
-    </row>
-    <row r="22" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="44"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="G22" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="H22" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="I22" s="20">
-        <v>0.7</v>
-      </c>
-      <c r="J22" s="47"/>
-    </row>
-    <row r="23" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="44"/>
-      <c r="C23" s="46">
-        <v>5</v>
-      </c>
-      <c r="D23" s="55" t="s">
+      <c r="D35" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="30" t="s">
-        <v>17</v>
+      <c r="E35" s="30" t="s">
+        <v>13</v>
       </c>
-      <c r="F23" s="50" t="s">
-        <v>18</v>
+      <c r="F35" s="46"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="48"/>
+      <c r="J35" s="49"/>
+    </row>
+    <row r="36" spans="2:10" s="27" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="45"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="50"/>
+    </row>
+    <row r="37" spans="2:10" s="27" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="45"/>
+      <c r="C37" s="49">
+        <v>12</v>
       </c>
-      <c r="G23" s="53"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="46"/>
-    </row>
-    <row r="24" spans="2:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="44"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="G24" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="H24" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="I24" s="20">
-        <v>0.7</v>
-      </c>
-      <c r="J24" s="47"/>
-    </row>
-    <row r="25" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="44"/>
-      <c r="C25" s="46">
-        <v>6</v>
-      </c>
-      <c r="D25" s="55" t="s">
+      <c r="D37" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="30" t="s">
-        <v>17</v>
+      <c r="E37" s="30" t="s">
+        <v>13</v>
       </c>
-      <c r="F25" s="50" t="s">
-        <v>18</v>
+      <c r="F37" s="46"/>
+      <c r="G37" s="47"/>
+      <c r="H37" s="47"/>
+      <c r="I37" s="48"/>
+      <c r="J37" s="49"/>
+    </row>
+    <row r="38" spans="2:10" s="27" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="45"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="52"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="50"/>
+    </row>
+    <row r="39" spans="2:10" s="27" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="45"/>
+      <c r="C39" s="49">
+        <v>13</v>
       </c>
-      <c r="G25" s="53"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="46"/>
-    </row>
-    <row r="26" spans="2:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="44"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="G26" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="H26" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="I26" s="20">
-        <v>0.7</v>
-      </c>
-      <c r="J26" s="47"/>
-    </row>
-    <row r="27" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="44"/>
-      <c r="C27" s="46">
-        <v>7</v>
-      </c>
-      <c r="D27" s="55" t="s">
+      <c r="D39" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="E27" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="G27" s="53"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="54"/>
-      <c r="J27" s="46"/>
-    </row>
-    <row r="28" spans="2:10" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="44"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="G28" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="H28" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="I28" s="20">
-        <v>0.7</v>
-      </c>
-      <c r="J28" s="47"/>
-    </row>
-    <row r="29" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="44"/>
-      <c r="C29" s="46">
-        <v>8</v>
-      </c>
-      <c r="D29" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="F29" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="52"/>
-      <c r="J29" s="46"/>
-    </row>
-    <row r="30" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="44"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F30" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="G30" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="H30" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="I30" s="20">
-        <v>0.7</v>
-      </c>
-      <c r="J30" s="56"/>
-    </row>
-    <row r="31" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="44"/>
-      <c r="C31" s="46">
-        <v>9</v>
-      </c>
-      <c r="D31" s="55" t="s">
-        <v>27</v>
-      </c>
-      <c r="E31" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="F31" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="G31" s="53"/>
-      <c r="H31" s="53"/>
-      <c r="I31" s="54"/>
-      <c r="J31" s="46"/>
-    </row>
-    <row r="32" spans="2:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="44"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="49"/>
-      <c r="E32" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="G32" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="H32" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="I32" s="20">
-        <v>0.7</v>
-      </c>
-      <c r="J32" s="47"/>
-    </row>
-    <row r="33" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="44"/>
-      <c r="C33" s="46">
-        <v>10</v>
-      </c>
-      <c r="D33" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="E33" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="F33" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="G33" s="53"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="54"/>
-      <c r="J33" s="46"/>
-    </row>
-    <row r="34" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="44"/>
-      <c r="C34" s="47"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F34" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="G34" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="H34" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="I34" s="20">
-        <v>0.7</v>
-      </c>
-      <c r="J34" s="47"/>
-    </row>
-    <row r="35" spans="2:10" s="27" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="45"/>
-      <c r="C35" s="46">
-        <v>11</v>
-      </c>
-      <c r="D35" s="57" t="s">
-        <v>29</v>
-      </c>
-      <c r="E35" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="F35" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="G35" s="53"/>
-      <c r="H35" s="53"/>
-      <c r="I35" s="54"/>
-      <c r="J35" s="46"/>
-    </row>
-    <row r="36" spans="2:10" s="27" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="45"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="58"/>
-      <c r="E36" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F36" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="G36" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="H36" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="I36" s="20">
-        <v>0.7</v>
-      </c>
-      <c r="J36" s="47"/>
-    </row>
-    <row r="37" spans="2:10" s="27" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="45"/>
-      <c r="C37" s="46">
-        <v>12</v>
-      </c>
-      <c r="D37" s="57" t="s">
-        <v>30</v>
-      </c>
-      <c r="E37" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="F37" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="G37" s="53"/>
-      <c r="H37" s="53"/>
-      <c r="I37" s="54"/>
-      <c r="J37" s="46"/>
-    </row>
-    <row r="38" spans="2:10" s="27" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="45"/>
-      <c r="C38" s="56"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F38" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="G38" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="H38" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="I38" s="20">
-        <v>0.7</v>
-      </c>
-      <c r="J38" s="47"/>
-    </row>
-    <row r="39" spans="2:10" s="27" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="45"/>
-      <c r="C39" s="46">
+      <c r="E39" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D39" s="57" t="s">
-        <v>31</v>
-      </c>
-      <c r="E39" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="F39" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="G39" s="53"/>
-      <c r="H39" s="53"/>
-      <c r="I39" s="54"/>
-      <c r="J39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="47"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="49"/>
     </row>
-    <row r="40" spans="2:10" s="27" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" s="27" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="45"/>
-      <c r="C40" s="56"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F40" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="G40" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="H40" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="I40" s="20">
-        <v>0.7</v>
-      </c>
-      <c r="J40" s="47"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="52"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="J39:J40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="J35:J36"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="J37:J38"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="J31:J32"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="J29:J30"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
     <mergeCell ref="C37:C38"/>
     <mergeCell ref="C39:C40"/>
     <mergeCell ref="F1:I1"/>
@@ -2246,34 +2094,23 @@
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="J15:J16"/>
     <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="J31:J32"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="J39:J40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="J35:J36"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="J37:J38"/>
   </mergeCells>
   <conditionalFormatting sqref="J2">
     <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Controlla se hai cancellato tutte le voci che non servono e se hai dato tutte le risposte">
@@ -2300,24 +2137,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:LI116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="189" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="189" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="14.453125" style="31"/>
-    <col min="3" max="3" width="6.36328125" style="31" customWidth="1"/>
-    <col min="4" max="4" width="68.6328125" style="31" customWidth="1"/>
-    <col min="5" max="5" width="6.1796875" style="31" customWidth="1"/>
-    <col min="6" max="7" width="14.453125" style="31"/>
+    <col min="1" max="2" width="14.42578125" style="31"/>
+    <col min="3" max="3" width="6.42578125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="68.5703125" style="31" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" style="31" customWidth="1"/>
+    <col min="6" max="7" width="14.42578125" style="31"/>
     <col min="8" max="8" width="14" style="31" customWidth="1"/>
     <col min="9" max="9" width="16" style="31" customWidth="1"/>
-    <col min="10" max="10" width="73.6328125" style="31" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="14.453125" style="31"/>
+    <col min="10" max="10" width="73.5703125" style="31" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="14.42578125" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="38.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" ht="38.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
       <c r="D1" s="34" t="s">
@@ -2326,40 +2163,40 @@
       <c r="E1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="59" t="s">
+      <c r="F1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="61"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="58"/>
       <c r="J1" s="36" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B2" s="44"/>
       <c r="C2" s="44"/>
       <c r="D2" s="8">
         <f>COUNTIF(E15:E64, "SI")</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E2" s="5">
         <f>COUNTIF(E15:E64, "NA")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
-      <c r="F2" s="62">
+      <c r="F2" s="59">
         <f>COUNTIF(F15:I64, "NO")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
       <c r="J2" s="9" t="str">
         <f>IF((D2+E2+F2)=53, OK, "Controlla se hai cancellato tutte le voci che non servono e se hai dato tutte le risposte")</f>
         <v>Controlla se hai cancellato tutte le voci che non servono e se hai dato tutte le risposte</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="45"/>
       <c r="C3" s="45"/>
       <c r="D3" s="10"/>
@@ -2380,7 +2217,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="45"/>
       <c r="C4" s="45"/>
       <c r="D4" s="11"/>
@@ -2401,12 +2238,12 @@
         <f>COUNTIF(F15:I64, I3)</f>
         <v>0</v>
       </c>
-      <c r="J4" s="9" t="str">
+      <c r="J4" s="9" t="e">
         <f>IF((F4+G4+H4)=(F2), OK, "Controlla se hai cancellato tutte le voci che non servono")</f>
-        <v>Controlla se hai cancellato tutte le voci che non servono</v>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B5" s="45"/>
       <c r="C5" s="45"/>
       <c r="D5" s="45"/>
@@ -2417,20 +2254,20 @@
       <c r="I5" s="45"/>
       <c r="J5" s="45"/>
     </row>
-    <row r="6" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="45"/>
       <c r="C6" s="45"/>
-      <c r="D6" s="79" t="s">
+      <c r="D6" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="80"/>
-      <c r="F6" s="80"/>
-      <c r="G6" s="80"/>
-      <c r="H6" s="80"/>
-      <c r="I6" s="80"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="78"/>
+      <c r="I6" s="78"/>
       <c r="J6" s="45"/>
     </row>
-    <row r="8" spans="2:10" ht="20" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:10" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B8" s="45"/>
       <c r="C8" s="45"/>
       <c r="D8" s="1" t="s">
@@ -2443,7 +2280,7 @@
       <c r="I8" s="45"/>
       <c r="J8" s="45"/>
     </row>
-    <row r="9" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B9" s="44"/>
       <c r="C9" s="44"/>
       <c r="D9" s="44"/>
@@ -2454,124 +2291,124 @@
       <c r="I9" s="44"/>
       <c r="J9" s="44"/>
     </row>
-    <row r="10" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:10" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="44"/>
-      <c r="C10" s="77" t="s">
-        <v>7</v>
+      <c r="C10" s="75" t="s">
+        <v>53</v>
       </c>
-      <c r="D10" s="78"/>
-      <c r="E10" s="72" t="s">
-        <v>8</v>
+      <c r="D10" s="76"/>
+      <c r="E10" s="70" t="s">
+        <v>54</v>
       </c>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="74"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="72"/>
       <c r="J10" s="2" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:10" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="44"/>
-      <c r="C11" s="71" t="s">
-        <v>10</v>
+      <c r="C11" s="69">
+        <v>1</v>
       </c>
-      <c r="D11" s="71"/>
+      <c r="D11" s="69"/>
       <c r="E11" s="38"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="81"/>
-      <c r="I11" s="81"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="79"/>
       <c r="J11" s="32"/>
     </row>
-    <row r="12" spans="2:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B12" s="44"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="76"/>
-      <c r="I12" s="76"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="74"/>
+      <c r="I12" s="74"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="44"/>
       <c r="C13" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
-      <c r="E13" s="65" t="s">
+      <c r="E13" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="44"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="85" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="85"/>
+      <c r="F14" s="85"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="85"/>
+      <c r="I14" s="85"/>
+      <c r="J14" s="86"/>
+    </row>
+    <row r="15" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="44"/>
+      <c r="C15" s="49">
+        <v>1</v>
+      </c>
+      <c r="D15" s="67" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="F15" s="80"/>
+      <c r="G15" s="81"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="49"/>
     </row>
-    <row r="14" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="44"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="117" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="117"/>
-      <c r="F14" s="117"/>
-      <c r="G14" s="117"/>
-      <c r="H14" s="117"/>
-      <c r="I14" s="117"/>
-      <c r="J14" s="118"/>
-    </row>
-    <row r="15" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="44"/>
-      <c r="C15" s="46">
-        <v>1</v>
-      </c>
-      <c r="D15" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="82"/>
-      <c r="G15" s="83"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="46"/>
-    </row>
-    <row r="16" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="45"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="70"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="68"/>
       <c r="E16" s="42"/>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
       <c r="I16" s="20"/>
-      <c r="J16" s="47"/>
+      <c r="J16" s="50"/>
     </row>
-    <row r="17" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="45"/>
       <c r="B17" s="44"/>
-      <c r="C17" s="46">
+      <c r="C17" s="49">
         <v>2</v>
       </c>
-      <c r="D17" s="48" t="s">
-        <v>34</v>
+      <c r="D17" s="67" t="s">
+        <v>28</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="F17" s="50"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="55"/>
+      <c r="J17" s="49"/>
       <c r="K17" s="45"/>
       <c r="L17" s="45"/>
       <c r="M17" s="45"/>
@@ -2884,17 +2721,17 @@
       <c r="LH17" s="45"/>
       <c r="LI17" s="45"/>
     </row>
-    <row r="18" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="45"/>
       <c r="B18" s="44"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="49"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="83"/>
       <c r="E18" s="26"/>
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="20"/>
-      <c r="J18" s="47"/>
+      <c r="J18" s="50"/>
       <c r="K18" s="45"/>
       <c r="L18" s="45"/>
       <c r="M18" s="45"/>
@@ -3207,22 +3044,22 @@
       <c r="LH18" s="45"/>
       <c r="LI18" s="45"/>
     </row>
-    <row r="19" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="45"/>
       <c r="B19" s="44"/>
-      <c r="C19" s="46">
+      <c r="C19" s="49">
         <v>3</v>
       </c>
-      <c r="D19" s="55" t="s">
-        <v>35</v>
+      <c r="D19" s="84" t="s">
+        <v>29</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="F19" s="50"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="52"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="55"/>
       <c r="J19" s="41"/>
       <c r="K19" s="45"/>
       <c r="L19" s="45"/>
@@ -3536,11 +3373,11 @@
       <c r="LH19" s="45"/>
       <c r="LI19" s="45"/>
     </row>
-    <row r="20" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="45"/>
       <c r="B20" s="44"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="49"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="83"/>
       <c r="E20" s="26"/>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
@@ -3859,23 +3696,23 @@
       <c r="LH20" s="45"/>
       <c r="LI20" s="45"/>
     </row>
-    <row r="21" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="45"/>
       <c r="B21" s="44"/>
-      <c r="C21" s="46">
+      <c r="C21" s="49">
         <v>4</v>
       </c>
-      <c r="D21" s="55" t="s">
-        <v>36</v>
+      <c r="D21" s="84" t="s">
+        <v>30</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="F21" s="50"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="49"/>
       <c r="K21" s="45"/>
       <c r="L21" s="45"/>
       <c r="M21" s="45"/>
@@ -4188,17 +4025,17 @@
       <c r="LH21" s="45"/>
       <c r="LI21" s="45"/>
     </row>
-    <row r="22" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="45"/>
       <c r="B22" s="44"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="49"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="83"/>
       <c r="E22" s="26"/>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
       <c r="H22" s="20"/>
       <c r="I22" s="20"/>
-      <c r="J22" s="47"/>
+      <c r="J22" s="50"/>
       <c r="K22" s="45"/>
       <c r="L22" s="45"/>
       <c r="M22" s="45"/>
@@ -4511,23 +4348,23 @@
       <c r="LH22" s="45"/>
       <c r="LI22" s="45"/>
     </row>
-    <row r="23" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="45"/>
       <c r="B23" s="44"/>
-      <c r="C23" s="46">
+      <c r="C23" s="49">
         <v>5</v>
       </c>
-      <c r="D23" s="55" t="s">
-        <v>37</v>
+      <c r="D23" s="84" t="s">
+        <v>31</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="F23" s="50"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="49"/>
       <c r="K23" s="45"/>
       <c r="L23" s="45"/>
       <c r="M23" s="45"/>
@@ -4840,17 +4677,17 @@
       <c r="LH23" s="45"/>
       <c r="LI23" s="45"/>
     </row>
-    <row r="24" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="45"/>
       <c r="B24" s="44"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="49"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="83"/>
       <c r="E24" s="26"/>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
       <c r="I24" s="20"/>
-      <c r="J24" s="47"/>
+      <c r="J24" s="50"/>
       <c r="K24" s="45"/>
       <c r="L24" s="45"/>
       <c r="M24" s="45"/>
@@ -5163,23 +5000,23 @@
       <c r="LH24" s="45"/>
       <c r="LI24" s="45"/>
     </row>
-    <row r="25" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="45"/>
       <c r="B25" s="44"/>
-      <c r="C25" s="46">
+      <c r="C25" s="49">
         <v>6</v>
       </c>
-      <c r="D25" s="55" t="s">
-        <v>38</v>
+      <c r="D25" s="84" t="s">
+        <v>32</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="F25" s="50"/>
-      <c r="G25" s="53"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="49"/>
       <c r="K25" s="45"/>
       <c r="L25" s="45"/>
       <c r="M25" s="45"/>
@@ -5492,17 +5329,17 @@
       <c r="LH25" s="45"/>
       <c r="LI25" s="45"/>
     </row>
-    <row r="26" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="45"/>
       <c r="B26" s="44"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="49"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="83"/>
       <c r="E26" s="18"/>
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
       <c r="I26" s="20"/>
-      <c r="J26" s="47"/>
+      <c r="J26" s="50"/>
       <c r="K26" s="45"/>
       <c r="L26" s="45"/>
       <c r="M26" s="45"/>
@@ -5815,19 +5652,19 @@
       <c r="LH26" s="45"/>
       <c r="LI26" s="45"/>
     </row>
-    <row r="27" spans="1:321" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:321" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="45"/>
       <c r="B27" s="45"/>
       <c r="C27" s="17"/>
-      <c r="D27" s="114" t="s">
-        <v>39</v>
+      <c r="D27" s="87" t="s">
+        <v>33</v>
       </c>
-      <c r="E27" s="115"/>
-      <c r="F27" s="115"/>
-      <c r="G27" s="115"/>
-      <c r="H27" s="115"/>
-      <c r="I27" s="115"/>
-      <c r="J27" s="116"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="88"/>
+      <c r="G27" s="88"/>
+      <c r="H27" s="88"/>
+      <c r="I27" s="88"/>
+      <c r="J27" s="89"/>
       <c r="K27" s="45"/>
       <c r="L27" s="45"/>
       <c r="M27" s="45"/>
@@ -6140,23 +5977,23 @@
       <c r="LH27" s="45"/>
       <c r="LI27" s="45"/>
     </row>
-    <row r="28" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="45"/>
       <c r="B28" s="45"/>
-      <c r="C28" s="105">
+      <c r="C28" s="90">
         <v>7</v>
       </c>
-      <c r="D28" s="111" t="s">
-        <v>40</v>
+      <c r="D28" s="93" t="s">
+        <v>34</v>
       </c>
       <c r="E28" s="39" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="F28" s="50"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="54"/>
-      <c r="J28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="49"/>
       <c r="K28" s="45"/>
       <c r="L28" s="45"/>
       <c r="M28" s="45"/>
@@ -6469,17 +6306,17 @@
       <c r="LH28" s="45"/>
       <c r="LI28" s="45"/>
     </row>
-    <row r="29" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="45"/>
       <c r="B29" s="45"/>
-      <c r="C29" s="106"/>
-      <c r="D29" s="112"/>
+      <c r="C29" s="91"/>
+      <c r="D29" s="94"/>
       <c r="E29" s="40"/>
       <c r="F29" s="20"/>
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
-      <c r="J29" s="47"/>
+      <c r="J29" s="50"/>
       <c r="K29" s="45"/>
       <c r="L29" s="45"/>
       <c r="M29" s="45"/>
@@ -6792,23 +6629,23 @@
       <c r="LH29" s="45"/>
       <c r="LI29" s="45"/>
     </row>
-    <row r="30" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="45"/>
       <c r="B30" s="45"/>
-      <c r="C30" s="105">
+      <c r="C30" s="90">
         <v>8</v>
       </c>
-      <c r="D30" s="110" t="s">
-        <v>41</v>
+      <c r="D30" s="92" t="s">
+        <v>35</v>
       </c>
       <c r="E30" s="39" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="F30" s="50"/>
-      <c r="G30" s="53"/>
-      <c r="H30" s="53"/>
-      <c r="I30" s="54"/>
-      <c r="J30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="49"/>
       <c r="K30" s="45"/>
       <c r="L30" s="45"/>
       <c r="M30" s="45"/>
@@ -7121,17 +6958,17 @@
       <c r="LH30" s="45"/>
       <c r="LI30" s="45"/>
     </row>
-    <row r="31" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="45"/>
       <c r="B31" s="45"/>
-      <c r="C31" s="106"/>
-      <c r="D31" s="58"/>
+      <c r="C31" s="91"/>
+      <c r="D31" s="52"/>
       <c r="E31" s="40"/>
       <c r="F31" s="20"/>
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
-      <c r="J31" s="47"/>
+      <c r="J31" s="50"/>
       <c r="K31" s="45"/>
       <c r="L31" s="45"/>
       <c r="M31" s="45"/>
@@ -7444,23 +7281,23 @@
       <c r="LH31" s="45"/>
       <c r="LI31" s="45"/>
     </row>
-    <row r="32" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="45"/>
       <c r="B32" s="45"/>
-      <c r="C32" s="105">
+      <c r="C32" s="90">
         <v>9</v>
       </c>
-      <c r="D32" s="110" t="s">
-        <v>42</v>
+      <c r="D32" s="92" t="s">
+        <v>36</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="F32" s="50"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="54"/>
-      <c r="J32" s="46"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="49"/>
       <c r="K32" s="45"/>
       <c r="L32" s="45"/>
       <c r="M32" s="45"/>
@@ -7773,17 +7610,17 @@
       <c r="LH32" s="45"/>
       <c r="LI32" s="45"/>
     </row>
-    <row r="33" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="45"/>
       <c r="B33" s="45"/>
-      <c r="C33" s="106"/>
-      <c r="D33" s="58"/>
+      <c r="C33" s="91"/>
+      <c r="D33" s="52"/>
       <c r="E33" s="26"/>
       <c r="F33" s="20"/>
       <c r="G33" s="20"/>
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
-      <c r="J33" s="47"/>
+      <c r="J33" s="50"/>
       <c r="K33" s="45"/>
       <c r="L33" s="45"/>
       <c r="M33" s="45"/>
@@ -8096,23 +7933,23 @@
       <c r="LH33" s="45"/>
       <c r="LI33" s="45"/>
     </row>
-    <row r="34" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="45"/>
       <c r="B34" s="45"/>
-      <c r="C34" s="105">
+      <c r="C34" s="90">
         <v>10</v>
       </c>
-      <c r="D34" s="57" t="s">
-        <v>43</v>
+      <c r="D34" s="51" t="s">
+        <v>37</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="F34" s="50"/>
-      <c r="G34" s="53"/>
-      <c r="H34" s="53"/>
-      <c r="I34" s="54"/>
-      <c r="J34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="47"/>
+      <c r="I34" s="48"/>
+      <c r="J34" s="49"/>
       <c r="K34" s="45"/>
       <c r="L34" s="45"/>
       <c r="M34" s="45"/>
@@ -8425,17 +8262,17 @@
       <c r="LH34" s="45"/>
       <c r="LI34" s="45"/>
     </row>
-    <row r="35" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="45"/>
       <c r="B35" s="45"/>
-      <c r="C35" s="106"/>
-      <c r="D35" s="58"/>
+      <c r="C35" s="91"/>
+      <c r="D35" s="52"/>
       <c r="E35" s="26"/>
       <c r="F35" s="20"/>
       <c r="G35" s="20"/>
       <c r="H35" s="20"/>
       <c r="I35" s="20"/>
-      <c r="J35" s="47"/>
+      <c r="J35" s="50"/>
       <c r="K35" s="45"/>
       <c r="L35" s="45"/>
       <c r="M35" s="45"/>
@@ -8748,23 +8585,23 @@
       <c r="LH35" s="45"/>
       <c r="LI35" s="45"/>
     </row>
-    <row r="36" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="45"/>
       <c r="B36" s="45"/>
-      <c r="C36" s="105">
+      <c r="C36" s="90">
         <v>11</v>
       </c>
-      <c r="D36" s="57" t="s">
-        <v>44</v>
+      <c r="D36" s="51" t="s">
+        <v>38</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="F36" s="50"/>
-      <c r="G36" s="53"/>
-      <c r="H36" s="53"/>
-      <c r="I36" s="54"/>
-      <c r="J36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="47"/>
+      <c r="H36" s="47"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="49"/>
       <c r="K36" s="45"/>
       <c r="L36" s="45"/>
       <c r="M36" s="45"/>
@@ -9077,17 +8914,17 @@
       <c r="LH36" s="45"/>
       <c r="LI36" s="45"/>
     </row>
-    <row r="37" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="45"/>
       <c r="B37" s="45"/>
-      <c r="C37" s="106"/>
-      <c r="D37" s="113"/>
+      <c r="C37" s="91"/>
+      <c r="D37" s="101"/>
       <c r="E37" s="26"/>
       <c r="F37" s="20"/>
       <c r="G37" s="20"/>
       <c r="H37" s="20"/>
       <c r="I37" s="20"/>
-      <c r="J37" s="47"/>
+      <c r="J37" s="50"/>
       <c r="K37" s="45"/>
       <c r="L37" s="45"/>
       <c r="M37" s="45"/>
@@ -9400,23 +9237,23 @@
       <c r="LH37" s="45"/>
       <c r="LI37" s="45"/>
     </row>
-    <row r="38" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="45"/>
       <c r="B38" s="44"/>
-      <c r="C38" s="105">
+      <c r="C38" s="90">
         <v>12</v>
       </c>
-      <c r="D38" s="110" t="s">
-        <v>45</v>
+      <c r="D38" s="92" t="s">
+        <v>39</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="F38" s="82"/>
-      <c r="G38" s="83"/>
-      <c r="H38" s="83"/>
-      <c r="I38" s="84"/>
-      <c r="J38" s="89"/>
+      <c r="F38" s="80"/>
+      <c r="G38" s="81"/>
+      <c r="H38" s="81"/>
+      <c r="I38" s="82"/>
+      <c r="J38" s="95"/>
       <c r="K38" s="45"/>
       <c r="L38" s="45"/>
       <c r="M38" s="45"/>
@@ -9729,17 +9566,17 @@
       <c r="LH38" s="45"/>
       <c r="LI38" s="45"/>
     </row>
-    <row r="39" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="45"/>
       <c r="B39" s="45"/>
-      <c r="C39" s="106"/>
-      <c r="D39" s="58"/>
+      <c r="C39" s="91"/>
+      <c r="D39" s="52"/>
       <c r="E39" s="22"/>
       <c r="F39" s="20"/>
       <c r="G39" s="20"/>
       <c r="H39" s="20"/>
       <c r="I39" s="20"/>
-      <c r="J39" s="90"/>
+      <c r="J39" s="96"/>
       <c r="K39" s="45"/>
       <c r="L39" s="45"/>
       <c r="M39" s="45"/>
@@ -10052,23 +9889,23 @@
       <c r="LH39" s="45"/>
       <c r="LI39" s="45"/>
     </row>
-    <row r="40" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="45"/>
       <c r="B40" s="44"/>
-      <c r="C40" s="105">
+      <c r="C40" s="90">
         <v>13</v>
       </c>
-      <c r="D40" s="85" t="s">
-        <v>46</v>
+      <c r="D40" s="97" t="s">
+        <v>40</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="F40" s="50"/>
-      <c r="G40" s="87"/>
-      <c r="H40" s="87"/>
-      <c r="I40" s="88"/>
-      <c r="J40" s="89"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="99"/>
+      <c r="H40" s="99"/>
+      <c r="I40" s="100"/>
+      <c r="J40" s="95"/>
       <c r="K40" s="45"/>
       <c r="L40" s="45"/>
       <c r="M40" s="45"/>
@@ -10381,17 +10218,17 @@
       <c r="LH40" s="45"/>
       <c r="LI40" s="45"/>
     </row>
-    <row r="41" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="45"/>
       <c r="B41" s="44"/>
-      <c r="C41" s="106"/>
-      <c r="D41" s="86"/>
+      <c r="C41" s="91"/>
+      <c r="D41" s="98"/>
       <c r="E41" s="22"/>
       <c r="F41" s="20"/>
       <c r="G41" s="20"/>
       <c r="H41" s="20"/>
       <c r="I41" s="20"/>
-      <c r="J41" s="90"/>
+      <c r="J41" s="96"/>
       <c r="K41" s="45"/>
       <c r="L41" s="45"/>
       <c r="M41" s="45"/>
@@ -10704,173 +10541,173 @@
       <c r="LH41" s="45"/>
       <c r="LI41" s="45"/>
     </row>
-    <row r="42" spans="1:321" s="29" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:321" s="29" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="28"/>
-      <c r="C42" s="105">
+      <c r="C42" s="90">
         <v>14</v>
       </c>
-      <c r="D42" s="85" t="s">
-        <v>47</v>
+      <c r="D42" s="97" t="s">
+        <v>41</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="F42" s="102"/>
-      <c r="G42" s="103"/>
-      <c r="H42" s="103"/>
-      <c r="I42" s="104"/>
-      <c r="J42" s="97"/>
+      <c r="F42" s="104"/>
+      <c r="G42" s="105"/>
+      <c r="H42" s="105"/>
+      <c r="I42" s="106"/>
+      <c r="J42" s="107"/>
     </row>
-    <row r="43" spans="1:321" s="29" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C43" s="106"/>
-      <c r="D43" s="86"/>
+    <row r="43" spans="1:321" s="29" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C43" s="91"/>
+      <c r="D43" s="98"/>
       <c r="E43" s="22"/>
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
       <c r="H43" s="21"/>
       <c r="I43" s="21"/>
-      <c r="J43" s="98"/>
+      <c r="J43" s="108"/>
     </row>
-    <row r="44" spans="1:321" s="29" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:321" s="29" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="28"/>
-      <c r="C44" s="105">
+      <c r="C44" s="90">
         <v>15</v>
       </c>
-      <c r="D44" s="92" t="s">
-        <v>48</v>
+      <c r="D44" s="102" t="s">
+        <v>42</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="F44" s="102"/>
-      <c r="G44" s="103"/>
-      <c r="H44" s="103"/>
-      <c r="I44" s="104"/>
-      <c r="J44" s="97"/>
+      <c r="F44" s="104"/>
+      <c r="G44" s="105"/>
+      <c r="H44" s="105"/>
+      <c r="I44" s="106"/>
+      <c r="J44" s="107"/>
     </row>
-    <row r="45" spans="1:321" s="29" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C45" s="106"/>
-      <c r="D45" s="101"/>
+    <row r="45" spans="1:321" s="29" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C45" s="91"/>
+      <c r="D45" s="103"/>
       <c r="E45" s="22"/>
       <c r="F45" s="21"/>
       <c r="G45" s="21"/>
       <c r="H45" s="21"/>
       <c r="I45" s="21"/>
-      <c r="J45" s="98"/>
+      <c r="J45" s="108"/>
     </row>
-    <row r="46" spans="1:321" s="29" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:321" s="29" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="28"/>
       <c r="C46" s="33"/>
-      <c r="D46" s="107" t="s">
-        <v>49</v>
+      <c r="D46" s="109" t="s">
+        <v>43</v>
       </c>
-      <c r="E46" s="108"/>
-      <c r="F46" s="108"/>
-      <c r="G46" s="108"/>
-      <c r="H46" s="108"/>
-      <c r="I46" s="108"/>
-      <c r="J46" s="109"/>
+      <c r="E46" s="110"/>
+      <c r="F46" s="110"/>
+      <c r="G46" s="110"/>
+      <c r="H46" s="110"/>
+      <c r="I46" s="110"/>
+      <c r="J46" s="111"/>
     </row>
-    <row r="47" spans="1:321" s="29" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:321" s="29" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="28"/>
-      <c r="C47" s="46">
+      <c r="C47" s="49">
         <v>16</v>
       </c>
-      <c r="D47" s="92" t="s">
-        <v>50</v>
+      <c r="D47" s="102" t="s">
+        <v>44</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="F47" s="102"/>
-      <c r="G47" s="103"/>
-      <c r="H47" s="103"/>
-      <c r="I47" s="104"/>
-      <c r="J47" s="97"/>
+      <c r="F47" s="104"/>
+      <c r="G47" s="105"/>
+      <c r="H47" s="105"/>
+      <c r="I47" s="106"/>
+      <c r="J47" s="107"/>
     </row>
-    <row r="48" spans="1:321" s="29" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C48" s="47"/>
-      <c r="D48" s="101"/>
+    <row r="48" spans="1:321" s="29" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C48" s="50"/>
+      <c r="D48" s="103"/>
       <c r="E48" s="22"/>
       <c r="F48" s="21"/>
       <c r="G48" s="21"/>
       <c r="H48" s="21"/>
       <c r="I48" s="21"/>
-      <c r="J48" s="98"/>
+      <c r="J48" s="108"/>
     </row>
-    <row r="49" spans="1:321" s="29" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:321" s="29" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="28"/>
-      <c r="C49" s="46">
+      <c r="C49" s="49">
         <v>17</v>
       </c>
-      <c r="D49" s="92" t="s">
-        <v>51</v>
+      <c r="D49" s="102" t="s">
+        <v>45</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="F49" s="94"/>
-      <c r="G49" s="95"/>
-      <c r="H49" s="95"/>
-      <c r="I49" s="96"/>
-      <c r="J49" s="97"/>
+      <c r="F49" s="114"/>
+      <c r="G49" s="115"/>
+      <c r="H49" s="115"/>
+      <c r="I49" s="116"/>
+      <c r="J49" s="107"/>
     </row>
-    <row r="50" spans="1:321" s="29" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:321" s="29" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="28"/>
-      <c r="C50" s="47"/>
-      <c r="D50" s="93"/>
+      <c r="C50" s="50"/>
+      <c r="D50" s="113"/>
       <c r="E50" s="22"/>
       <c r="F50" s="21"/>
       <c r="G50" s="21"/>
       <c r="H50" s="21"/>
       <c r="I50" s="21"/>
-      <c r="J50" s="98"/>
+      <c r="J50" s="108"/>
     </row>
-    <row r="51" spans="1:321" s="29" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:321" s="29" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="28"/>
-      <c r="C51" s="46">
+      <c r="C51" s="49">
         <v>18</v>
       </c>
-      <c r="D51" s="99" t="s">
-        <v>52</v>
+      <c r="D51" s="117" t="s">
+        <v>46</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="F51" s="94"/>
-      <c r="G51" s="95"/>
-      <c r="H51" s="95"/>
-      <c r="I51" s="96"/>
-      <c r="J51" s="97"/>
+      <c r="F51" s="114"/>
+      <c r="G51" s="115"/>
+      <c r="H51" s="115"/>
+      <c r="I51" s="116"/>
+      <c r="J51" s="107"/>
     </row>
-    <row r="52" spans="1:321" s="29" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:321" s="29" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="28"/>
-      <c r="C52" s="47"/>
-      <c r="D52" s="100"/>
+      <c r="C52" s="50"/>
+      <c r="D52" s="118"/>
       <c r="E52" s="22"/>
       <c r="F52" s="21"/>
       <c r="G52" s="21"/>
       <c r="H52" s="21"/>
       <c r="I52" s="21"/>
-      <c r="J52" s="98"/>
+      <c r="J52" s="108"/>
     </row>
-    <row r="53" spans="1:321" s="25" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:321" s="25" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="45"/>
       <c r="B53" s="44"/>
-      <c r="C53" s="46">
+      <c r="C53" s="49">
         <v>19</v>
       </c>
-      <c r="D53" s="85" t="s">
-        <v>53</v>
+      <c r="D53" s="97" t="s">
+        <v>47</v>
       </c>
       <c r="E53" s="22" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="F53" s="50"/>
-      <c r="G53" s="87"/>
-      <c r="H53" s="87"/>
-      <c r="I53" s="88"/>
-      <c r="J53" s="89"/>
+      <c r="F53" s="46"/>
+      <c r="G53" s="99"/>
+      <c r="H53" s="99"/>
+      <c r="I53" s="100"/>
+      <c r="J53" s="95"/>
       <c r="K53" s="45"/>
       <c r="L53" s="45"/>
       <c r="M53" s="45"/>
@@ -11183,17 +11020,17 @@
       <c r="LH53" s="45"/>
       <c r="LI53" s="45"/>
     </row>
-    <row r="54" spans="1:321" s="25" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:321" s="25" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="45"/>
       <c r="B54" s="44"/>
-      <c r="C54" s="47"/>
-      <c r="D54" s="86"/>
+      <c r="C54" s="50"/>
+      <c r="D54" s="98"/>
       <c r="E54" s="22"/>
       <c r="F54" s="20"/>
       <c r="G54" s="20"/>
       <c r="H54" s="20"/>
       <c r="I54" s="20"/>
-      <c r="J54" s="90"/>
+      <c r="J54" s="96"/>
       <c r="K54" s="45"/>
       <c r="L54" s="45"/>
       <c r="M54" s="45"/>
@@ -11506,23 +11343,23 @@
       <c r="LH54" s="45"/>
       <c r="LI54" s="45"/>
     </row>
-    <row r="55" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="45"/>
       <c r="B55" s="44"/>
-      <c r="C55" s="46">
+      <c r="C55" s="49">
         <v>20</v>
       </c>
-      <c r="D55" s="91" t="s">
-        <v>54</v>
+      <c r="D55" s="112" t="s">
+        <v>48</v>
       </c>
       <c r="E55" s="22" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="F55" s="50"/>
-      <c r="G55" s="87"/>
-      <c r="H55" s="87"/>
-      <c r="I55" s="88"/>
-      <c r="J55" s="89"/>
+      <c r="F55" s="46"/>
+      <c r="G55" s="99"/>
+      <c r="H55" s="99"/>
+      <c r="I55" s="100"/>
+      <c r="J55" s="95"/>
       <c r="K55" s="45"/>
       <c r="L55" s="45"/>
       <c r="M55" s="45"/>
@@ -11835,17 +11672,17 @@
       <c r="LH55" s="45"/>
       <c r="LI55" s="45"/>
     </row>
-    <row r="56" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="45"/>
       <c r="B56" s="44"/>
-      <c r="C56" s="47"/>
-      <c r="D56" s="86"/>
+      <c r="C56" s="50"/>
+      <c r="D56" s="98"/>
       <c r="E56" s="22"/>
       <c r="F56" s="20"/>
       <c r="G56" s="20"/>
       <c r="H56" s="20"/>
       <c r="I56" s="20"/>
-      <c r="J56" s="90"/>
+      <c r="J56" s="96"/>
       <c r="K56" s="45"/>
       <c r="L56" s="45"/>
       <c r="M56" s="45"/>
@@ -12158,23 +11995,23 @@
       <c r="LH56" s="45"/>
       <c r="LI56" s="45"/>
     </row>
-    <row r="57" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="45"/>
       <c r="B57" s="44"/>
-      <c r="C57" s="46">
+      <c r="C57" s="49">
         <v>21</v>
       </c>
-      <c r="D57" s="91" t="s">
-        <v>55</v>
+      <c r="D57" s="112" t="s">
+        <v>49</v>
       </c>
       <c r="E57" s="22" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="F57" s="50"/>
-      <c r="G57" s="87"/>
-      <c r="H57" s="87"/>
-      <c r="I57" s="88"/>
-      <c r="J57" s="89"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="99"/>
+      <c r="H57" s="99"/>
+      <c r="I57" s="100"/>
+      <c r="J57" s="95"/>
       <c r="K57" s="45"/>
       <c r="L57" s="45"/>
       <c r="M57" s="45"/>
@@ -12487,17 +12324,17 @@
       <c r="LH57" s="45"/>
       <c r="LI57" s="45"/>
     </row>
-    <row r="58" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="45"/>
       <c r="B58" s="44"/>
-      <c r="C58" s="47"/>
-      <c r="D58" s="86"/>
+      <c r="C58" s="50"/>
+      <c r="D58" s="98"/>
       <c r="E58" s="22"/>
       <c r="F58" s="20"/>
       <c r="G58" s="20"/>
       <c r="H58" s="20"/>
       <c r="I58" s="20"/>
-      <c r="J58" s="90"/>
+      <c r="J58" s="96"/>
       <c r="K58" s="45"/>
       <c r="L58" s="45"/>
       <c r="M58" s="45"/>
@@ -12810,23 +12647,23 @@
       <c r="LH58" s="45"/>
       <c r="LI58" s="45"/>
     </row>
-    <row r="59" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="45"/>
       <c r="B59" s="44"/>
-      <c r="C59" s="46">
+      <c r="C59" s="49">
         <v>22</v>
       </c>
-      <c r="D59" s="91" t="s">
-        <v>56</v>
+      <c r="D59" s="112" t="s">
+        <v>50</v>
       </c>
       <c r="E59" s="22" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="F59" s="50"/>
-      <c r="G59" s="87"/>
-      <c r="H59" s="87"/>
-      <c r="I59" s="88"/>
-      <c r="J59" s="89"/>
+      <c r="F59" s="46"/>
+      <c r="G59" s="99"/>
+      <c r="H59" s="99"/>
+      <c r="I59" s="100"/>
+      <c r="J59" s="95"/>
       <c r="K59" s="45"/>
       <c r="L59" s="45"/>
       <c r="M59" s="45"/>
@@ -13139,17 +12976,17 @@
       <c r="LH59" s="45"/>
       <c r="LI59" s="45"/>
     </row>
-    <row r="60" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="45"/>
       <c r="B60" s="44"/>
-      <c r="C60" s="47"/>
-      <c r="D60" s="86"/>
+      <c r="C60" s="50"/>
+      <c r="D60" s="98"/>
       <c r="E60" s="22"/>
       <c r="F60" s="20"/>
       <c r="G60" s="20"/>
       <c r="H60" s="20"/>
       <c r="I60" s="20"/>
-      <c r="J60" s="90"/>
+      <c r="J60" s="96"/>
       <c r="K60" s="45"/>
       <c r="L60" s="45"/>
       <c r="M60" s="45"/>
@@ -13462,23 +13299,25 @@
       <c r="LH60" s="45"/>
       <c r="LI60" s="45"/>
     </row>
-    <row r="61" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="45"/>
       <c r="B61" s="44"/>
-      <c r="C61" s="46">
+      <c r="C61" s="49">
         <v>23</v>
       </c>
-      <c r="D61" s="85" t="s">
-        <v>57</v>
+      <c r="D61" s="97" t="s">
+        <v>51</v>
       </c>
-      <c r="E61" s="22"/>
-      <c r="F61" s="50" t="s">
-        <v>18</v>
+      <c r="E61" s="22" t="s">
+        <v>13</v>
       </c>
-      <c r="G61" s="87"/>
-      <c r="H61" s="87"/>
-      <c r="I61" s="88"/>
-      <c r="J61" s="89"/>
+      <c r="F61" s="46"/>
+      <c r="G61" s="99"/>
+      <c r="H61" s="99"/>
+      <c r="I61" s="100"/>
+      <c r="J61" s="95" t="s">
+        <v>56</v>
+      </c>
       <c r="K61" s="45"/>
       <c r="L61" s="45"/>
       <c r="M61" s="45"/>
@@ -13791,19 +13630,17 @@
       <c r="LH61" s="45"/>
       <c r="LI61" s="45"/>
     </row>
-    <row r="62" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="45"/>
       <c r="B62" s="44"/>
-      <c r="C62" s="47"/>
-      <c r="D62" s="86"/>
-      <c r="E62" s="22" t="s">
-        <v>19</v>
-      </c>
+      <c r="C62" s="50"/>
+      <c r="D62" s="98"/>
+      <c r="E62" s="22"/>
       <c r="F62" s="20"/>
       <c r="G62" s="20"/>
       <c r="H62" s="20"/>
       <c r="I62" s="20"/>
-      <c r="J62" s="90"/>
+      <c r="J62" s="96"/>
       <c r="K62" s="45"/>
       <c r="L62" s="45"/>
       <c r="M62" s="45"/>
@@ -14116,23 +13953,23 @@
       <c r="LH62" s="45"/>
       <c r="LI62" s="45"/>
     </row>
-    <row r="63" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="45"/>
       <c r="B63" s="44"/>
-      <c r="C63" s="46">
+      <c r="C63" s="49">
         <v>24</v>
       </c>
-      <c r="D63" s="91" t="s">
-        <v>58</v>
+      <c r="D63" s="112" t="s">
+        <v>52</v>
       </c>
       <c r="E63" s="22" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="F63" s="50"/>
-      <c r="G63" s="87"/>
-      <c r="H63" s="87"/>
-      <c r="I63" s="88"/>
-      <c r="J63" s="89"/>
+      <c r="F63" s="46"/>
+      <c r="G63" s="99"/>
+      <c r="H63" s="99"/>
+      <c r="I63" s="100"/>
+      <c r="J63" s="95"/>
       <c r="K63" s="45"/>
       <c r="L63" s="45"/>
       <c r="M63" s="45"/>
@@ -14445,17 +14282,17 @@
       <c r="LH63" s="45"/>
       <c r="LI63" s="45"/>
     </row>
-    <row r="64" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:321" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="45"/>
       <c r="B64" s="44"/>
-      <c r="C64" s="47"/>
-      <c r="D64" s="86"/>
+      <c r="C64" s="50"/>
+      <c r="D64" s="98"/>
       <c r="E64" s="22"/>
       <c r="F64" s="20"/>
       <c r="G64" s="20"/>
       <c r="H64" s="20"/>
       <c r="I64" s="20"/>
-      <c r="J64" s="90"/>
+      <c r="J64" s="96"/>
       <c r="K64" s="45"/>
       <c r="L64" s="45"/>
       <c r="M64" s="45"/>
@@ -14768,7 +14605,7 @@
       <c r="LH64" s="45"/>
       <c r="LI64" s="45"/>
     </row>
-    <row r="65" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="45"/>
       <c r="B65" s="45"/>
       <c r="C65" s="45"/>
@@ -15091,7 +14928,7 @@
       <c r="LH65" s="45"/>
       <c r="LI65" s="45"/>
     </row>
-    <row r="66" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="45"/>
       <c r="B66" s="45"/>
       <c r="C66" s="45"/>
@@ -15414,7 +15251,7 @@
       <c r="LH66" s="45"/>
       <c r="LI66" s="45"/>
     </row>
-    <row r="67" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="45"/>
       <c r="B67" s="45"/>
       <c r="C67" s="45"/>
@@ -15737,7 +15574,7 @@
       <c r="LH67" s="45"/>
       <c r="LI67" s="45"/>
     </row>
-    <row r="68" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="45"/>
       <c r="B68" s="45"/>
       <c r="C68" s="45"/>
@@ -16060,7 +15897,7 @@
       <c r="LH68" s="45"/>
       <c r="LI68" s="45"/>
     </row>
-    <row r="69" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="45"/>
       <c r="B69" s="45"/>
       <c r="C69" s="45"/>
@@ -16383,7 +16220,7 @@
       <c r="LH69" s="45"/>
       <c r="LI69" s="45"/>
     </row>
-    <row r="70" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="45"/>
       <c r="B70" s="45"/>
       <c r="C70" s="45"/>
@@ -16706,7 +16543,7 @@
       <c r="LH70" s="45"/>
       <c r="LI70" s="45"/>
     </row>
-    <row r="71" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="45"/>
       <c r="B71" s="45"/>
       <c r="C71" s="45"/>
@@ -17029,7 +16866,7 @@
       <c r="LH71" s="45"/>
       <c r="LI71" s="45"/>
     </row>
-    <row r="72" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="45"/>
       <c r="B72" s="45"/>
       <c r="C72" s="45"/>
@@ -17352,7 +17189,7 @@
       <c r="LH72" s="45"/>
       <c r="LI72" s="45"/>
     </row>
-    <row r="73" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="45"/>
       <c r="B73" s="45"/>
       <c r="C73" s="45"/>
@@ -17675,7 +17512,7 @@
       <c r="LH73" s="45"/>
       <c r="LI73" s="45"/>
     </row>
-    <row r="74" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="45"/>
       <c r="B74" s="45"/>
       <c r="C74" s="45"/>
@@ -17998,7 +17835,7 @@
       <c r="LH74" s="45"/>
       <c r="LI74" s="45"/>
     </row>
-    <row r="75" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="45"/>
       <c r="B75" s="45"/>
       <c r="C75" s="45"/>
@@ -18321,7 +18158,7 @@
       <c r="LH75" s="45"/>
       <c r="LI75" s="45"/>
     </row>
-    <row r="76" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="45"/>
       <c r="B76" s="45"/>
       <c r="C76" s="45"/>
@@ -18644,7 +18481,7 @@
       <c r="LH76" s="45"/>
       <c r="LI76" s="45"/>
     </row>
-    <row r="77" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="45"/>
       <c r="B77" s="45"/>
       <c r="C77" s="45"/>
@@ -18967,7 +18804,7 @@
       <c r="LH77" s="45"/>
       <c r="LI77" s="45"/>
     </row>
-    <row r="78" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="45"/>
       <c r="B78" s="45"/>
       <c r="C78" s="45"/>
@@ -19290,7 +19127,7 @@
       <c r="LH78" s="45"/>
       <c r="LI78" s="45"/>
     </row>
-    <row r="79" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="45"/>
       <c r="B79" s="45"/>
       <c r="C79" s="45"/>
@@ -19613,7 +19450,7 @@
       <c r="LH79" s="45"/>
       <c r="LI79" s="45"/>
     </row>
-    <row r="80" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="45"/>
       <c r="B80" s="45"/>
       <c r="C80" s="45"/>
@@ -19936,7 +19773,7 @@
       <c r="LH80" s="45"/>
       <c r="LI80" s="45"/>
     </row>
-    <row r="81" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="45"/>
       <c r="B81" s="45"/>
       <c r="C81" s="45"/>
@@ -20259,7 +20096,7 @@
       <c r="LH81" s="45"/>
       <c r="LI81" s="45"/>
     </row>
-    <row r="82" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="45"/>
       <c r="B82" s="45"/>
       <c r="C82" s="45"/>
@@ -20582,7 +20419,7 @@
       <c r="LH82" s="45"/>
       <c r="LI82" s="45"/>
     </row>
-    <row r="83" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="45"/>
       <c r="B83" s="45"/>
       <c r="C83" s="45"/>
@@ -20905,7 +20742,7 @@
       <c r="LH83" s="45"/>
       <c r="LI83" s="45"/>
     </row>
-    <row r="84" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="45"/>
       <c r="B84" s="45"/>
       <c r="C84" s="45"/>
@@ -21228,7 +21065,7 @@
       <c r="LH84" s="45"/>
       <c r="LI84" s="45"/>
     </row>
-    <row r="85" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="45"/>
       <c r="B85" s="45"/>
       <c r="C85" s="45"/>
@@ -21551,7 +21388,7 @@
       <c r="LH85" s="45"/>
       <c r="LI85" s="45"/>
     </row>
-    <row r="86" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="45"/>
       <c r="B86" s="45"/>
       <c r="C86" s="45"/>
@@ -21874,7 +21711,7 @@
       <c r="LH86" s="45"/>
       <c r="LI86" s="45"/>
     </row>
-    <row r="87" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="45"/>
       <c r="B87" s="45"/>
       <c r="C87" s="45"/>
@@ -22197,7 +22034,7 @@
       <c r="LH87" s="45"/>
       <c r="LI87" s="45"/>
     </row>
-    <row r="88" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="45"/>
       <c r="B88" s="45"/>
       <c r="C88" s="45"/>
@@ -22520,7 +22357,7 @@
       <c r="LH88" s="45"/>
       <c r="LI88" s="45"/>
     </row>
-    <row r="89" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="45"/>
       <c r="B89" s="45"/>
       <c r="C89" s="45"/>
@@ -22843,7 +22680,7 @@
       <c r="LH89" s="45"/>
       <c r="LI89" s="45"/>
     </row>
-    <row r="90" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="45"/>
       <c r="B90" s="45"/>
       <c r="C90" s="45"/>
@@ -23166,7 +23003,7 @@
       <c r="LH90" s="45"/>
       <c r="LI90" s="45"/>
     </row>
-    <row r="91" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="45"/>
       <c r="B91" s="45"/>
       <c r="C91" s="45"/>
@@ -23489,7 +23326,7 @@
       <c r="LH91" s="45"/>
       <c r="LI91" s="45"/>
     </row>
-    <row r="92" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="45"/>
       <c r="B92" s="45"/>
       <c r="C92" s="45"/>
@@ -23812,7 +23649,7 @@
       <c r="LH92" s="45"/>
       <c r="LI92" s="45"/>
     </row>
-    <row r="93" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="45"/>
       <c r="B93" s="45"/>
       <c r="C93" s="45"/>
@@ -24135,7 +23972,7 @@
       <c r="LH93" s="45"/>
       <c r="LI93" s="45"/>
     </row>
-    <row r="94" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="45"/>
       <c r="B94" s="45"/>
       <c r="C94" s="45"/>
@@ -24458,7 +24295,7 @@
       <c r="LH94" s="45"/>
       <c r="LI94" s="45"/>
     </row>
-    <row r="95" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="45"/>
       <c r="B95" s="45"/>
       <c r="C95" s="45"/>
@@ -24781,7 +24618,7 @@
       <c r="LH95" s="45"/>
       <c r="LI95" s="45"/>
     </row>
-    <row r="96" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="45"/>
       <c r="B96" s="45"/>
       <c r="C96" s="45"/>
@@ -25104,7 +24941,7 @@
       <c r="LH96" s="45"/>
       <c r="LI96" s="45"/>
     </row>
-    <row r="97" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="45"/>
       <c r="B97" s="45"/>
       <c r="C97" s="45"/>
@@ -25427,7 +25264,7 @@
       <c r="LH97" s="45"/>
       <c r="LI97" s="45"/>
     </row>
-    <row r="98" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="45"/>
       <c r="B98" s="45"/>
       <c r="C98" s="45"/>
@@ -25750,7 +25587,7 @@
       <c r="LH98" s="45"/>
       <c r="LI98" s="45"/>
     </row>
-    <row r="99" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="45"/>
       <c r="B99" s="45"/>
       <c r="C99" s="45"/>
@@ -26073,7 +25910,7 @@
       <c r="LH99" s="45"/>
       <c r="LI99" s="45"/>
     </row>
-    <row r="100" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="45"/>
       <c r="B100" s="45"/>
       <c r="C100" s="45"/>
@@ -26396,7 +26233,7 @@
       <c r="LH100" s="45"/>
       <c r="LI100" s="45"/>
     </row>
-    <row r="101" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="45"/>
       <c r="B101" s="45"/>
       <c r="C101" s="45"/>
@@ -26719,7 +26556,7 @@
       <c r="LH101" s="45"/>
       <c r="LI101" s="45"/>
     </row>
-    <row r="102" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="45"/>
       <c r="B102" s="45"/>
       <c r="C102" s="45"/>
@@ -27042,7 +26879,7 @@
       <c r="LH102" s="45"/>
       <c r="LI102" s="45"/>
     </row>
-    <row r="103" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="45"/>
       <c r="B103" s="45"/>
       <c r="C103" s="45"/>
@@ -27365,7 +27202,7 @@
       <c r="LH103" s="45"/>
       <c r="LI103" s="45"/>
     </row>
-    <row r="104" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="45"/>
       <c r="B104" s="45"/>
       <c r="C104" s="45"/>
@@ -27688,7 +27525,7 @@
       <c r="LH104" s="45"/>
       <c r="LI104" s="45"/>
     </row>
-    <row r="105" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="45"/>
       <c r="B105" s="45"/>
       <c r="C105" s="45"/>
@@ -28011,7 +27848,7 @@
       <c r="LH105" s="45"/>
       <c r="LI105" s="45"/>
     </row>
-    <row r="106" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="45"/>
       <c r="B106" s="45"/>
       <c r="C106" s="45"/>
@@ -28334,7 +28171,7 @@
       <c r="LH106" s="45"/>
       <c r="LI106" s="45"/>
     </row>
-    <row r="107" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="45"/>
       <c r="B107" s="45"/>
       <c r="C107" s="45"/>
@@ -28657,7 +28494,7 @@
       <c r="LH107" s="45"/>
       <c r="LI107" s="45"/>
     </row>
-    <row r="108" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="45"/>
       <c r="B108" s="45"/>
       <c r="C108" s="45"/>
@@ -28980,7 +28817,7 @@
       <c r="LH108" s="45"/>
       <c r="LI108" s="45"/>
     </row>
-    <row r="109" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="45"/>
       <c r="B109" s="45"/>
       <c r="C109" s="45"/>
@@ -29303,7 +29140,7 @@
       <c r="LH109" s="45"/>
       <c r="LI109" s="45"/>
     </row>
-    <row r="110" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="45"/>
       <c r="B110" s="45"/>
       <c r="C110" s="45"/>
@@ -29626,7 +29463,7 @@
       <c r="LH110" s="45"/>
       <c r="LI110" s="45"/>
     </row>
-    <row r="111" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="45"/>
       <c r="B111" s="45"/>
       <c r="C111" s="45"/>
@@ -29949,7 +29786,7 @@
       <c r="LH111" s="45"/>
       <c r="LI111" s="45"/>
     </row>
-    <row r="112" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="45"/>
       <c r="B112" s="45"/>
       <c r="C112" s="45"/>
@@ -30272,7 +30109,7 @@
       <c r="LH112" s="45"/>
       <c r="LI112" s="45"/>
     </row>
-    <row r="113" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="45"/>
       <c r="B113" s="45"/>
       <c r="C113" s="45"/>
@@ -30595,7 +30432,7 @@
       <c r="LH113" s="45"/>
       <c r="LI113" s="45"/>
     </row>
-    <row r="114" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="45"/>
       <c r="B114" s="45"/>
       <c r="C114" s="45"/>
@@ -30918,7 +30755,7 @@
       <c r="LH114" s="45"/>
       <c r="LI114" s="45"/>
     </row>
-    <row r="115" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="45"/>
       <c r="B115" s="45"/>
       <c r="C115" s="45"/>
@@ -31241,7 +31078,7 @@
       <c r="LH115" s="45"/>
       <c r="LI115" s="45"/>
     </row>
-    <row r="116" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="45"/>
       <c r="B116" s="45"/>
       <c r="C116" s="45"/>
@@ -31566,44 +31403,51 @@
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="E12:I12"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="D14:J14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:I10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="D27:J27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="J61:J62"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="J63:J64"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="J57:J58"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="J59:J60"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="J53:J54"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="J55:J56"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="J49:J50"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="J51:J52"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="J47:J48"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="J44:J45"/>
+    <mergeCell ref="D46:J46"/>
     <mergeCell ref="D38:D39"/>
     <mergeCell ref="D30:D31"/>
     <mergeCell ref="D28:D29"/>
@@ -31628,51 +31472,44 @@
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="J32:J33"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="J47:J48"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="J44:J45"/>
-    <mergeCell ref="D46:J46"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="J53:J54"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="J55:J56"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="J49:J50"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="J51:J52"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="J61:J62"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="J63:J64"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="J57:J58"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="J59:J60"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="D27:J27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="E12:I12"/>
+    <mergeCell ref="E13:I13"/>
+    <mergeCell ref="D14:J14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:I10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:I11"/>
   </mergeCells>
   <conditionalFormatting sqref="J2">
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Controlla se hai cancellato tutte le voci che non servono e se hai dato tutte le risposte">

</xml_diff>